<commit_message>
Renamed worksheet to MessiGoals
</commit_message>
<xml_diff>
--- a/Excel/LionelMessiGoals_Clean.xlsx
+++ b/Excel/LionelMessiGoals_Clean.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\GitProjects\MessiGoalsExploration\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59649A9-CF73-4E3C-8834-8F2C1DF61E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7958A9FD-5AD1-49A7-B7CB-B5B63EB421CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="3120" windowWidth="28800" windowHeight="15910" xr2:uid="{26EE471C-8546-4D62-8601-7A5F55885B8C}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="LionelMessiGoals" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$L$705</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LionelMessiGoals!$A$1:$L$705</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>